<commit_message>
Update automatico via Actualizar 05-04-2020 19-49-48
</commit_message>
<xml_diff>
--- a/datacovidhn/LOCALIZA HN.xlsx
+++ b/datacovidhn/LOCALIZA HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\000 DRIVE\000 DATACOVID HN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{23A5930A-7705-4873-9354-6671A8986A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BD912FE3-1129-4ED5-9577-2DB3AE28073F}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{23A5930A-7705-4873-9354-6671A8986A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BC5F9EF6-C4D2-4F55-A4B0-9607C15AFDFC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E12A4D3B-4BD9-444E-BCAD-8267569BA124}"/>
   </bookViews>
@@ -4940,8 +4940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57166B67-A93A-452E-A5E0-8FB31F384F7A}">
   <dimension ref="A1:M299"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
+      <selection activeCell="J283" sqref="J283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -5038,7 +5038,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" ht="15">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -5075,7 +5075,7 @@
       <c r="L3" t="s">
         <v>25</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -16518,7 +16518,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="283" spans="1:13">
+    <row r="283" spans="1:13" ht="15">
       <c r="A283" t="s">
         <v>13</v>
       </c>
@@ -16555,7 +16555,7 @@
       <c r="L283" t="s">
         <v>1425</v>
       </c>
-      <c r="M283" t="s">
+      <c r="M283" s="1" t="s">
         <v>1426</v>
       </c>
     </row>
@@ -17218,10 +17218,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M2" r:id="rId1" xr:uid="{C1D39B31-F093-4443-8E56-AB312BD2C198}"/>
+    <hyperlink ref="M3" r:id="rId2" xr:uid="{7F9AC178-7925-462F-9377-1D53986C46B8}"/>
+    <hyperlink ref="M283" r:id="rId3" xr:uid="{4D56EABC-E703-43B9-9CE2-F8421E9FDAD3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 05-04-2020 20-24-31
</commit_message>
<xml_diff>
--- a/datacovidhn/LOCALIZA HN.xlsx
+++ b/datacovidhn/LOCALIZA HN.xlsx
@@ -4940,8 +4940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57166B67-A93A-452E-A5E0-8FB31F384F7A}">
   <dimension ref="A1:M299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
-      <selection activeCell="J283" sqref="J283"/>
+    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="J185" sqref="J185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-04-2020 20-39-05
</commit_message>
<xml_diff>
--- a/datacovidhn/LOCALIZA HN.xlsx
+++ b/datacovidhn/LOCALIZA HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\000 DRIVE\000 DATACOVID HN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{23A5930A-7705-4873-9354-6671A8986A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BC5F9EF6-C4D2-4F55-A4B0-9607C15AFDFC}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{23A5930A-7705-4873-9354-6671A8986A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2B10AFAF-D541-4A76-B81C-9F307AC6D393}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E12A4D3B-4BD9-444E-BCAD-8267569BA124}"/>
   </bookViews>
@@ -4940,8 +4940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57166B67-A93A-452E-A5E0-8FB31F384F7A}">
   <dimension ref="A1:M299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="J185" sqref="J185"/>
+    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
+      <selection activeCell="J286" sqref="J286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -12910,7 +12910,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="195" spans="1:13">
+    <row r="195" spans="1:13" ht="15">
       <c r="A195" t="s">
         <v>13</v>
       </c>
@@ -12947,7 +12947,7 @@
       <c r="L195" t="s">
         <v>989</v>
       </c>
-      <c r="M195" t="s">
+      <c r="M195" s="1" t="s">
         <v>990</v>
       </c>
     </row>
@@ -17220,10 +17220,11 @@
     <hyperlink ref="M2" r:id="rId1" xr:uid="{C1D39B31-F093-4443-8E56-AB312BD2C198}"/>
     <hyperlink ref="M3" r:id="rId2" xr:uid="{7F9AC178-7925-462F-9377-1D53986C46B8}"/>
     <hyperlink ref="M283" r:id="rId3" xr:uid="{4D56EABC-E703-43B9-9CE2-F8421E9FDAD3}"/>
+    <hyperlink ref="M195" r:id="rId4" xr:uid="{E090D897-0CBE-4BE0-8282-3A9A8B6C7557}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 05-04-2020 22-01-56
</commit_message>
<xml_diff>
--- a/datacovidhn/LOCALIZA HN.xlsx
+++ b/datacovidhn/LOCALIZA HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\000 DRIVE\000 DATACOVID HN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{23A5930A-7705-4873-9354-6671A8986A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2B10AFAF-D541-4A76-B81C-9F307AC6D393}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{23A5930A-7705-4873-9354-6671A8986A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{26896FD2-6F31-4E80-9A55-6CF3D12050A9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E12A4D3B-4BD9-444E-BCAD-8267569BA124}"/>
   </bookViews>
@@ -4940,8 +4940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57166B67-A93A-452E-A5E0-8FB31F384F7A}">
   <dimension ref="A1:M299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
-      <selection activeCell="J286" sqref="J286"/>
+    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="H205" sqref="H205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-04-2020 23-24-21
</commit_message>
<xml_diff>
--- a/datacovidhn/LOCALIZA HN.xlsx
+++ b/datacovidhn/LOCALIZA HN.xlsx
@@ -4940,8 +4940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57166B67-A93A-452E-A5E0-8FB31F384F7A}">
   <dimension ref="A1:M299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="H205" sqref="H205"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-08-2020 04-48-34
</commit_message>
<xml_diff>
--- a/datacovidhn/LOCALIZA HN.xlsx
+++ b/datacovidhn/LOCALIZA HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\000 DRIVE\000 DATACOVID HN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="13_ncr:1_{23A5930A-7705-4873-9354-6671A8986A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{014A3EE4-3DDA-4048-9ABA-7333DB8FEC70}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{23A5930A-7705-4873-9354-6671A8986A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B55EEB91-B0A5-4413-85B0-55724699CB64}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E12A4D3B-4BD9-444E-BCAD-8267569BA124}"/>
   </bookViews>
@@ -1505,6 +1505,9 @@
     <t>https://www.google.com/maps/place/Municipio de Danli + Departamento de El Paraiso + Honduras</t>
   </si>
   <si>
+    <t>0704</t>
+  </si>
+  <si>
     <t>HND-0704</t>
   </si>
   <si>
@@ -1941,9 +1944,6 @@
   </si>
   <si>
     <t>https://www.google.com/maps/place/Municipio de Orica + Departamento de Francisco Morazan + Honduras</t>
-  </si>
-  <si>
-    <t>0815</t>
   </si>
   <si>
     <t>Reitoca</t>
@@ -4937,8 +4937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57166B67-A93A-452E-A5E0-8FB31F384F7A}">
   <dimension ref="A1:M299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="G95" sqref="G95"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -8826,8 +8826,8 @@
       <c r="F95">
         <v>4</v>
       </c>
-      <c r="G95">
-        <v>704</v>
+      <c r="G95" t="s">
+        <v>490</v>
       </c>
       <c r="H95" t="s">
         <v>258</v>
@@ -8839,13 +8839,13 @@
         <v>-86.525899999999993</v>
       </c>
       <c r="K95" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="L95" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="M95" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="96" spans="1:13">
@@ -8868,10 +8868,10 @@
         <v>5</v>
       </c>
       <c r="G96" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="H96" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="I96">
         <v>13.8704</v>
@@ -8880,13 +8880,13 @@
         <v>-86.942999999999998</v>
       </c>
       <c r="K96" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="L96" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="M96" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="97" spans="1:13">
@@ -8909,10 +8909,10 @@
         <v>6</v>
       </c>
       <c r="G97" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="H97" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="I97">
         <v>14.0349</v>
@@ -8921,13 +8921,13 @@
         <v>-86.6768</v>
       </c>
       <c r="K97" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="L97" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="M97" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="98" spans="1:13">
@@ -8950,10 +8950,10 @@
         <v>7</v>
       </c>
       <c r="G98" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="H98" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="I98">
         <v>13.553699999999999</v>
@@ -8962,13 +8962,13 @@
         <v>-87.06</v>
       </c>
       <c r="K98" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="L98" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="M98" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="99" spans="1:13">
@@ -8991,10 +8991,10 @@
         <v>8</v>
       </c>
       <c r="G99" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="H99" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="I99">
         <v>14.148199999999999</v>
@@ -9003,13 +9003,13 @@
         <v>-86.853999999999999</v>
       </c>
       <c r="K99" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="L99" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="M99" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="100" spans="1:13">
@@ -9032,10 +9032,10 @@
         <v>9</v>
       </c>
       <c r="G100" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="H100" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="I100">
         <v>13.8195</v>
@@ -9044,13 +9044,13 @@
         <v>-86.833200000000005</v>
       </c>
       <c r="K100" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="L100" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="M100" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="101" spans="1:13">
@@ -9073,7 +9073,7 @@
         <v>10</v>
       </c>
       <c r="G101" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="H101" t="s">
         <v>354</v>
@@ -9085,13 +9085,13 @@
         <v>-86.756500000000003</v>
       </c>
       <c r="K101" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="L101" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="M101" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="102" spans="1:13">
@@ -9114,7 +9114,7 @@
         <v>11</v>
       </c>
       <c r="G102" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="H102" t="s">
         <v>450</v>
@@ -9126,13 +9126,13 @@
         <v>-86.839399999999998</v>
       </c>
       <c r="K102" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="L102" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="M102" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="103" spans="1:13">
@@ -9155,10 +9155,10 @@
         <v>12</v>
       </c>
       <c r="G103" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="H103" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="I103">
         <v>13.7478</v>
@@ -9167,13 +9167,13 @@
         <v>-86.948599999999999</v>
       </c>
       <c r="K103" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="L103" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="M103" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="104" spans="1:13">
@@ -9196,10 +9196,10 @@
         <v>13</v>
       </c>
       <c r="G104" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="H104" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="I104">
         <v>13.958</v>
@@ -9208,13 +9208,13 @@
         <v>-86.647999999999996</v>
       </c>
       <c r="K104" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="L104" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="M104" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="105" spans="1:13">
@@ -9237,10 +9237,10 @@
         <v>14</v>
       </c>
       <c r="G105" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="H105" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="I105">
         <v>13.614699999999999</v>
@@ -9249,13 +9249,13 @@
         <v>-87.147099999999995</v>
       </c>
       <c r="K105" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="L105" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="M105" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="106" spans="1:13">
@@ -9278,10 +9278,10 @@
         <v>15</v>
       </c>
       <c r="G106" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="H106" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="I106">
         <v>14.295199999999999</v>
@@ -9290,13 +9290,13 @@
         <v>-86.679000000000002</v>
       </c>
       <c r="K106" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="L106" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M106" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="107" spans="1:13">
@@ -9319,10 +9319,10 @@
         <v>16</v>
       </c>
       <c r="G107" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="H107" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="I107">
         <v>13.6693</v>
@@ -9331,13 +9331,13 @@
         <v>-87.038600000000002</v>
       </c>
       <c r="K107" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="L107" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="M107" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="108" spans="1:13">
@@ -9360,10 +9360,10 @@
         <v>17</v>
       </c>
       <c r="G108" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="H108" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="I108">
         <v>13.639699999999999</v>
@@ -9372,13 +9372,13 @@
         <v>-86.954499999999996</v>
       </c>
       <c r="K108" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="L108" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="M108" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="109" spans="1:13">
@@ -9401,10 +9401,10 @@
         <v>18</v>
       </c>
       <c r="G109" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="H109" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="I109">
         <v>13.751099999999999</v>
@@ -9413,13 +9413,13 @@
         <v>-87.079599999999999</v>
       </c>
       <c r="K109" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="L109" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="M109" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="110" spans="1:13">
@@ -9442,10 +9442,10 @@
         <v>19</v>
       </c>
       <c r="G110" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="H110" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="I110">
         <v>14.045299999999999</v>
@@ -9454,13 +9454,13 @@
         <v>-85.860699999999994</v>
       </c>
       <c r="K110" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="L110" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="M110" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="111" spans="1:13">
@@ -9474,19 +9474,19 @@
         <v>8</v>
       </c>
       <c r="D111" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E111" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F111">
         <v>1</v>
       </c>
       <c r="G111" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H111" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="I111">
         <v>14.175800000000001</v>
@@ -9495,13 +9495,13 @@
         <v>-87.251099999999994</v>
       </c>
       <c r="K111" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="L111" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="M111" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="112" spans="1:13">
@@ -9515,19 +9515,19 @@
         <v>8</v>
       </c>
       <c r="D112" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E112" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F112">
         <v>2</v>
       </c>
       <c r="G112" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="H112" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="I112">
         <v>13.786300000000001</v>
@@ -9536,13 +9536,13 @@
         <v>-87.470699999999994</v>
       </c>
       <c r="K112" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="L112" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="M112" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="113" spans="1:13">
@@ -9556,19 +9556,19 @@
         <v>8</v>
       </c>
       <c r="D113" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E113" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F113">
         <v>3</v>
       </c>
       <c r="G113" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="H113" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="I113">
         <v>14.57</v>
@@ -9577,13 +9577,13 @@
         <v>-87.121499999999997</v>
       </c>
       <c r="K113" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="L113" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="M113" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="114" spans="1:13">
@@ -9597,19 +9597,19 @@
         <v>8</v>
       </c>
       <c r="D114" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E114" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F114">
         <v>4</v>
       </c>
       <c r="G114" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H114" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="I114">
         <v>13.8278</v>
@@ -9618,13 +9618,13 @@
         <v>-87.568700000000007</v>
       </c>
       <c r="K114" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="L114" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="M114" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="115" spans="1:13">
@@ -9638,16 +9638,16 @@
         <v>8</v>
       </c>
       <c r="D115" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E115" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F115">
         <v>5</v>
       </c>
       <c r="G115" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="H115" t="s">
         <v>23</v>
@@ -9659,13 +9659,13 @@
         <v>-87.221999999999994</v>
       </c>
       <c r="K115" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="L115" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="M115" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="116" spans="1:13">
@@ -9679,19 +9679,19 @@
         <v>8</v>
       </c>
       <c r="D116" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E116" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F116">
         <v>6</v>
       </c>
       <c r="G116" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="H116" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="I116">
         <v>14.513299999999999</v>
@@ -9700,13 +9700,13 @@
         <v>-86.867800000000003</v>
       </c>
       <c r="K116" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="L116" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="M116" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="117" spans="1:13">
@@ -9720,16 +9720,16 @@
         <v>8</v>
       </c>
       <c r="D117" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E117" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F117">
         <v>7</v>
       </c>
       <c r="G117" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="H117" t="s">
         <v>136</v>
@@ -9741,13 +9741,13 @@
         <v>-87.500500000000002</v>
       </c>
       <c r="K117" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="L117" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="M117" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="118" spans="1:13">
@@ -9761,19 +9761,19 @@
         <v>8</v>
       </c>
       <c r="D118" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E118" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F118">
         <v>8</v>
       </c>
       <c r="G118" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="H118" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="I118">
         <v>13.732100000000001</v>
@@ -9782,13 +9782,13 @@
         <v>-87.327600000000004</v>
       </c>
       <c r="K118" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="L118" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="M118" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="119" spans="1:13">
@@ -9802,19 +9802,19 @@
         <v>8</v>
       </c>
       <c r="D119" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E119" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F119">
         <v>9</v>
       </c>
       <c r="G119" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="H119" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="I119">
         <v>14.0482</v>
@@ -9823,13 +9823,13 @@
         <v>-87.495500000000007</v>
       </c>
       <c r="K119" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="L119" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="M119" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="120" spans="1:13">
@@ -9843,19 +9843,19 @@
         <v>8</v>
       </c>
       <c r="D120" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E120" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F120">
         <v>10</v>
       </c>
       <c r="G120" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="H120" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="I120">
         <v>13.8675</v>
@@ -9864,13 +9864,13 @@
         <v>-87.056399999999996</v>
       </c>
       <c r="K120" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="L120" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="M120" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="121" spans="1:13">
@@ -9884,19 +9884,19 @@
         <v>8</v>
       </c>
       <c r="D121" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E121" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F121">
         <v>11</v>
       </c>
       <c r="G121" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="H121" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="I121">
         <v>14.938000000000001</v>
@@ -9905,13 +9905,13 @@
         <v>-87.102400000000003</v>
       </c>
       <c r="K121" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="L121" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="M121" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="122" spans="1:13">
@@ -9925,19 +9925,19 @@
         <v>8</v>
       </c>
       <c r="D122" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E122" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F122">
         <v>12</v>
       </c>
       <c r="G122" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="H122" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="I122">
         <v>13.7515</v>
@@ -9946,13 +9946,13 @@
         <v>-87.1614</v>
       </c>
       <c r="K122" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="L122" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="M122" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="123" spans="1:13">
@@ -9966,19 +9966,19 @@
         <v>8</v>
       </c>
       <c r="D123" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E123" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F123">
         <v>13</v>
       </c>
       <c r="G123" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="H123" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="I123">
         <v>13.9277</v>
@@ -9987,13 +9987,13 @@
         <v>-87.340999999999994</v>
       </c>
       <c r="K123" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="L123" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="M123" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="124" spans="1:13">
@@ -10007,19 +10007,19 @@
         <v>8</v>
       </c>
       <c r="D124" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E124" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F124">
         <v>14</v>
       </c>
       <c r="G124" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="H124" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="I124">
         <v>14.797800000000001</v>
@@ -10028,13 +10028,13 @@
         <v>-86.945400000000006</v>
       </c>
       <c r="K124" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="L124" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="M124" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="125" spans="1:13">
@@ -10048,16 +10048,16 @@
         <v>8</v>
       </c>
       <c r="D125" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E125" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F125">
         <v>15</v>
       </c>
-      <c r="G125" t="s">
-        <v>636</v>
+      <c r="G125">
+        <v>815</v>
       </c>
       <c r="H125" t="s">
         <v>637</v>
@@ -10089,10 +10089,10 @@
         <v>8</v>
       </c>
       <c r="D126" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E126" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F126">
         <v>16</v>
@@ -10130,10 +10130,10 @@
         <v>8</v>
       </c>
       <c r="D127" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E127" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F127">
         <v>17</v>
@@ -10171,10 +10171,10 @@
         <v>8</v>
       </c>
       <c r="D128" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E128" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F128">
         <v>18</v>
@@ -10212,10 +10212,10 @@
         <v>8</v>
       </c>
       <c r="D129" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E129" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F129">
         <v>19</v>
@@ -10253,10 +10253,10 @@
         <v>8</v>
       </c>
       <c r="D130" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E130" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F130">
         <v>20</v>
@@ -10294,10 +10294,10 @@
         <v>8</v>
       </c>
       <c r="D131" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E131" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F131">
         <v>21</v>
@@ -10335,10 +10335,10 @@
         <v>8</v>
       </c>
       <c r="D132" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E132" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F132">
         <v>22</v>
@@ -10376,10 +10376,10 @@
         <v>8</v>
       </c>
       <c r="D133" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E133" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F133">
         <v>23</v>
@@ -10417,10 +10417,10 @@
         <v>8</v>
       </c>
       <c r="D134" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E134" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F134">
         <v>24</v>
@@ -10458,10 +10458,10 @@
         <v>8</v>
       </c>
       <c r="D135" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E135" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F135">
         <v>25</v>
@@ -10499,10 +10499,10 @@
         <v>8</v>
       </c>
       <c r="D136" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E136" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F136">
         <v>26</v>
@@ -10540,10 +10540,10 @@
         <v>8</v>
       </c>
       <c r="D137" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E137" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F137">
         <v>27</v>
@@ -10581,10 +10581,10 @@
         <v>8</v>
       </c>
       <c r="D138" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E138" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F138">
         <v>28</v>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-08-2020 06-11-01
</commit_message>
<xml_diff>
--- a/datacovidhn/LOCALIZA HN.xlsx
+++ b/datacovidhn/LOCALIZA HN.xlsx
@@ -4937,8 +4937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57166B67-A93A-452E-A5E0-8FB31F384F7A}">
   <dimension ref="A1:M299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-12-2020 00-49-30
</commit_message>
<xml_diff>
--- a/datacovidhn/LOCALIZA HN.xlsx
+++ b/datacovidhn/LOCALIZA HN.xlsx
@@ -4934,8 +4934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57166B67-A93A-452E-A5E0-8FB31F384F7A}">
   <dimension ref="A1:M299"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
+      <selection activeCell="G302" sqref="G302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-15-2020 15-04-50
</commit_message>
<xml_diff>
--- a/datacovidhn/LOCALIZA HN.xlsx
+++ b/datacovidhn/LOCALIZA HN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22904"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\000 DRIVE\000 DATACOVID HN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="13_ncr:1_{23A5930A-7705-4873-9354-6671A8986A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D3BDC38E-FFAB-46A3-A142-FC4BA000E58A}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="13_ncr:1_{23A5930A-7705-4873-9354-6671A8986A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{694996BE-CAB8-444C-AD3D-9AA614815163}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E12A4D3B-4BD9-444E-BCAD-8267569BA124}"/>
   </bookViews>
@@ -4934,8 +4934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57166B67-A93A-452E-A5E0-8FB31F384F7A}">
   <dimension ref="A1:M299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
-      <selection activeCell="G302" sqref="G302"/>
+    <sheetView tabSelected="1" topLeftCell="E66" workbookViewId="0">
+      <selection activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -4945,7 +4945,7 @@
     <col min="5" max="5" width="16.140625" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" customWidth="1"/>
     <col min="12" max="12" width="16.28515625" customWidth="1"/>
   </cols>

</xml_diff>